<commit_message>
Fixed result  path display.
</commit_message>
<xml_diff>
--- a/aMaze_ingSolver/Results.xlsx
+++ b/aMaze_ingSolver/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vojtěch\Source\Repos\aMAZEing\aMaze_ingSolver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E48DB352-0C08-4EED-860A-8B757A2711E9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1AD8BBCF-05B1-4873-8584-98685F4FA775}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{9C37580C-5007-48F2-A604-DB6C7B31C129}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="17">
   <si>
     <t>Převod obrázku na matici</t>
   </si>
@@ -66,13 +66,16 @@
     <t>Depth firsts</t>
   </si>
   <si>
-    <t>Dijkstra firsts</t>
-  </si>
-  <si>
-    <t>A* firsts</t>
-  </si>
-  <si>
-    <t>NON-DEF</t>
+    <t>NDF</t>
+  </si>
+  <si>
+    <t>KAZDE MERENI PRUMER 3</t>
+  </si>
+  <si>
+    <t>Dijkstra</t>
+  </si>
+  <si>
+    <t>A*</t>
   </si>
 </sst>
 </file>
@@ -109,9 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -426,15 +430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2813EB67-3091-4FD9-9AF7-76DAB44EF997}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
     <col min="2" max="2" width="27.109375" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5546875" customWidth="1"/>
@@ -569,6 +573,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -584,264 +591,444 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>15</v>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
-        <v>15</v>
+      <c r="C11" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="F12" t="s">
-        <v>15</v>
+      <c r="C12" s="2">
+        <v>6.05</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2">
+        <v>15.1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
-        <v>15</v>
+      <c r="C13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1230</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>64</v>
-      </c>
-      <c r="F14" t="s">
-        <v>15</v>
-      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F15" t="s">
-        <v>15</v>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="F16" t="s">
-        <v>15</v>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
-        <v>15</v>
+      <c r="C17" s="2">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="E17" s="2">
+        <v>6</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="F18" t="s">
-        <v>15</v>
+      <c r="C18" s="2">
+        <v>23.3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E18" s="2">
+        <v>18.3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="F19" t="s">
-        <v>15</v>
+      <c r="C19" s="2">
+        <v>356</v>
+      </c>
+      <c r="D19" s="2">
+        <v>323</v>
+      </c>
+      <c r="E19" s="2">
+        <v>290.60000000000002</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="F20" t="s">
-        <v>15</v>
+      <c r="C20" s="2">
+        <v>673</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1894</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1388</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>5328</v>
-      </c>
-      <c r="D21">
-        <v>2996</v>
-      </c>
-      <c r="E21">
-        <v>9270</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F22" t="s">
-        <v>15</v>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="F23" t="s">
-        <v>15</v>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
-        <v>15</v>
+      <c r="C24" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D24" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>6</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="F25" t="s">
-        <v>15</v>
+      <c r="C25" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="D25" s="2">
+        <v>21.3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>20</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="F26" t="s">
-        <v>15</v>
+      <c r="C26" s="2">
+        <v>339</v>
+      </c>
+      <c r="D26" s="2">
+        <v>347</v>
+      </c>
+      <c r="E26" s="2">
+        <v>318</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="F27" t="s">
-        <v>15</v>
+      <c r="C27" s="2">
+        <v>753</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2055</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" t="s">
-        <v>15</v>
-      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F29" t="s">
-        <v>15</v>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" t="s">
         <v>15</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="F31" t="s">
-        <v>15</v>
+      <c r="C31" s="2">
+        <v>36</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>2</v>
       </c>
-      <c r="F32" t="s">
-        <v>15</v>
+      <c r="C32" s="2">
+        <v>272</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
-      <c r="F33" t="s">
-        <v>15</v>
+      <c r="C33" s="2">
+        <v>32791</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="F34" t="s">
-        <v>15</v>
+      <c r="C34" s="2">
+        <v>20868</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" t="s">
-        <v>15</v>
-      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F36" t="s">
-        <v>15</v>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1</v>
       </c>
+      <c r="C38">
+        <v>45</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>2</v>
       </c>
+      <c r="C39">
+        <v>237</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>8</v>
       </c>
+      <c r="C40">
+        <v>39234</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
       <c r="F40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>3</v>
       </c>
+      <c r="C41">
+        <v>24151</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
       <c r="F41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>